<commit_message>
DOCS: math ops matrix updated, showing corrections required.
</commit_message>
<xml_diff>
--- a/docs/math-ops-matrix.xlsx
+++ b/docs/math-ops-matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27602" windowHeight="13844" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27600" windowHeight="13845" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Red Math Ops (current)" sheetId="6" r:id="rId1"/>
@@ -14,7 +14,6 @@
   <customWorkbookViews>
     <customWorkbookView name="dk - Personal View" guid="{6590DA0F-755E-492A-8B86-272A49DB945C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1461" windowHeight="848" activeSheetId="1"/>
   </customWorkbookViews>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -109,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="13">
   <si>
     <t>integer!</t>
   </si>
@@ -146,6 +145,9 @@
   <si>
     <t>time! 
 float!</t>
+  </si>
+  <si>
+    <t>To be done</t>
   </si>
 </sst>
 </file>
@@ -192,7 +194,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,6 +210,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,7 +271,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -305,6 +313,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1459,18 +1473,18 @@
   <dimension ref="B3:N15"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="9" width="11.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="9" width="11.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:14" ht="41.2" customHeight="1">
+    <row r="3" spans="2:14" ht="41.25" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1709,18 +1723,19 @@
   <dimension ref="B3:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="9" width="11.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="9" width="11.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:14" ht="41.2" customHeight="1">
+    <row r="3" spans="2:14" ht="41.25" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1817,7 +1832,9 @@
       <c r="G6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="5"/>
+      <c r="H6" s="14" t="s">
+        <v>6</v>
+      </c>
       <c r="I6" s="7" t="s">
         <v>3</v>
       </c>
@@ -1831,9 +1848,7 @@
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="C7" s="14"/>
       <c r="D7" s="7" t="s">
         <v>8</v>
       </c>
@@ -1844,21 +1859,23 @@
         <v>8</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="7" t="s">
         <v>3</v>
       </c>
       <c r="J7" s="5"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="2:14" ht="43.5" customHeight="1">
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="C8" s="14"/>
       <c r="D8" s="7" t="s">
         <v>1</v>
       </c>
@@ -1883,7 +1900,9 @@
       <c r="D9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="14" t="s">
+        <v>6</v>
+      </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="8" t="s">

</xml_diff>

<commit_message>
DOCS: minor update of the math ops matrix.
Just marking the implemented cases.
</commit_message>
<xml_diff>
--- a/docs/math-ops-matrix.xlsx
+++ b/docs/math-ops-matrix.xlsx
@@ -1723,7 +1723,7 @@
   <dimension ref="B3:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C7" sqref="C7:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1848,7 +1848,7 @@
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="7" t="s">
         <v>8</v>
       </c>
@@ -1875,7 +1875,7 @@
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="7" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
DOCS: applied all pending changes.
</commit_message>
<xml_diff>
--- a/docs/math-ops-matrix.xlsx
+++ b/docs/math-ops-matrix.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27600" windowHeight="13845" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27602" windowHeight="13844" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Red Math Ops (current)" sheetId="6" r:id="rId1"/>
-    <sheet name="Red Math Ops (target)" sheetId="1" r:id="rId2"/>
+    <sheet name="Red Math Ops (old)" sheetId="6" r:id="rId1"/>
+    <sheet name="Red Math Ops" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
   <customWorkbookViews>
@@ -108,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="12">
   <si>
     <t>integer!</t>
   </si>
@@ -145,9 +146,6 @@
   <si>
     <t>time! 
 float!</t>
-  </si>
-  <si>
-    <t>To be done</t>
   </si>
 </sst>
 </file>
@@ -194,7 +192,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,14 +211,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -265,13 +257,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -314,10 +326,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1473,18 +1488,18 @@
   <dimension ref="B3:N15"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="9" width="11.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="3" max="9" width="11.875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:14" ht="41.25" customHeight="1">
+    <row r="3" spans="2:14" ht="41.2" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1723,19 +1738,19 @@
   <dimension ref="B3:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C8"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="9" width="11.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="3" max="9" width="11.875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.25" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:14" ht="41.25" customHeight="1">
+    <row r="3" spans="2:14" ht="41.2" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1832,14 +1847,14 @@
       <c r="G6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="J6" s="5"/>
-      <c r="L6" s="12"/>
+      <c r="L6" s="15"/>
       <c r="M6" s="6" t="s">
         <v>5</v>
       </c>
@@ -1861,15 +1876,15 @@
       <c r="G7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="5"/>
+      <c r="H7" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="I7" s="7" t="s">
         <v>3</v>
       </c>
       <c r="J7" s="5"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="L7" s="16"/>
+      <c r="M7" s="14"/>
     </row>
     <row r="8" spans="2:14" ht="43.5" customHeight="1">
       <c r="B8" s="4" t="s">
@@ -1900,10 +1915,12 @@
       <c r="D9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="8" t="s">
         <v>6</v>
@@ -1978,4 +1995,16 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
FEAT: updates math ops matrix.
Numbers/Vector ops allowed.
Pair & Tuple operations with Vector forbidden. (those types do not fit the vector storage model)
Unimplemented cases marked as such.
</commit_message>
<xml_diff>
--- a/docs/math-ops-matrix.xlsx
+++ b/docs/math-ops-matrix.xlsx
@@ -4,12 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27602" windowHeight="13844" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27600" windowHeight="13845"/>
   </bookViews>
   <sheets>
-    <sheet name="Red Math Ops (old)" sheetId="6" r:id="rId1"/>
-    <sheet name="Red Math Ops" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId3"/>
+    <sheet name="Red Math Ops" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
   <customWorkbookViews>
@@ -63,53 +61,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>dk</author>
-  </authors>
-  <commentList>
-    <comment ref="G8" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>dk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">time  + - // %  time     -&gt;      time            *
-time     /          time      -&gt;      float
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="13">
   <si>
     <t>integer!</t>
   </si>
@@ -146,6 +99,9 @@
   <si>
     <t>time! 
 float!</t>
+  </si>
+  <si>
+    <t>Not implemented yet</t>
   </si>
 </sst>
 </file>
@@ -192,7 +148,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,8 +167,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -268,22 +230,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -326,14 +279,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1487,19 +1443,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:N15"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="9" width="11.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="9" width="11.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:14" ht="41.2" customHeight="1">
+    <row r="3" spans="2:14" ht="41.25" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1545,7 +1503,9 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+      <c r="J4" s="15" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="2:14" ht="43.5" customHeight="1">
       <c r="B5" s="4" t="s">
@@ -1572,7 +1532,9 @@
       <c r="I5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="5"/>
+      <c r="J5" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="L5" s="13"/>
       <c r="M5" s="10"/>
       <c r="N5" s="11"/>
@@ -1596,12 +1558,16 @@
       <c r="G6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="5"/>
+      <c r="H6" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="I6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="5"/>
-      <c r="L6" s="12"/>
+      <c r="J6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="14"/>
       <c r="M6" s="6" t="s">
         <v>5</v>
       </c>
@@ -1610,9 +1576,7 @@
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="C7" s="12"/>
       <c r="D7" s="7" t="s">
         <v>8</v>
       </c>
@@ -1623,21 +1587,27 @@
         <v>8</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="I7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="5"/>
+      <c r="J7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="16"/>
+      <c r="M7" s="17" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="2:14" ht="43.5" customHeight="1">
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="C8" s="12"/>
       <c r="D8" s="7" t="s">
         <v>1</v>
       </c>
@@ -1652,7 +1622,9 @@
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+      <c r="J8" s="15" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="2:14" ht="43.5" customHeight="1">
       <c r="B9" s="4" t="s">
@@ -1662,8 +1634,12 @@
       <c r="D9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="E9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="8" t="s">
         <v>6</v>
@@ -1696,7 +1672,7 @@
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -1708,272 +1684,11 @@
       <c r="F11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14">
-      <c r="B15" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:N15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
-  <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="9" width="11.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.25" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:14" ht="41.2" customHeight="1">
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" ht="43.5" customHeight="1">
-      <c r="B4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="2:14" ht="43.5" customHeight="1">
-      <c r="B5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="5"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="11"/>
-    </row>
-    <row r="6" spans="2:14" ht="43.5" customHeight="1">
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J6" s="5"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" ht="43.5" customHeight="1">
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" s="5"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="14"/>
-    </row>
-    <row r="8" spans="2:14" ht="43.5" customHeight="1">
-      <c r="B8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="2:14" ht="43.5" customHeight="1">
-      <c r="B9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="2:14" ht="43.5" customHeight="1">
-      <c r="B10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="2:14" ht="43.5" customHeight="1">
-      <c r="B11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>4</v>
-      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
       <c r="J11" s="8" t="s">
         <v>4</v>
       </c>
@@ -1995,16 +1710,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>